<commit_message>
Initial commit of secondaries
</commit_message>
<xml_diff>
--- a/SecondariesList.xlsx
+++ b/SecondariesList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3560" yWindow="-21600" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AMCAS" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="66">
   <si>
     <t>Med School</t>
   </si>
@@ -228,6 +228,9 @@
   </si>
   <si>
     <t>Please describe any personal experiences or disadvantage (educational, financial or otherwise) and their significance to you in your pursuit of a medical degree. If not applicable, please so indicate. (300 words)</t>
+  </si>
+  <si>
+    <t>https://studentaffairs.swmed.org/mygateway/login.aspx</t>
   </si>
 </sst>
 </file>
@@ -381,14 +384,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -764,40 +767,40 @@
     <row r="3" spans="1:4" s="8" customFormat="1">
       <c r="A3" s="19"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="23"/>
+      <c r="C3" s="21"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="32">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="22" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="23" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16">
-      <c r="A5" s="21"/>
+      <c r="A5" s="22"/>
       <c r="C5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="22"/>
+      <c r="D5" s="23"/>
     </row>
     <row r="6" spans="1:4" ht="16">
-      <c r="A6" s="21"/>
+      <c r="A6" s="22"/>
       <c r="C6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="22"/>
+      <c r="D6" s="23"/>
     </row>
     <row r="7" spans="1:4" ht="30">
-      <c r="A7" s="21"/>
+      <c r="A7" s="22"/>
       <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="22"/>
+      <c r="D7" s="23"/>
     </row>
     <row r="8" spans="1:4" s="8" customFormat="1">
       <c r="A8" s="19"/>
@@ -806,7 +809,7 @@
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="99" customHeight="1">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="22" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -817,7 +820,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="30">
-      <c r="A10" s="21"/>
+      <c r="A10" s="22"/>
       <c r="C10" s="2" t="s">
         <v>8</v>
       </c>
@@ -826,7 +829,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="240">
-      <c r="A11" s="21"/>
+      <c r="A11" s="22"/>
       <c r="C11" s="2" t="s">
         <v>19</v>
       </c>
@@ -835,7 +838,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="30">
-      <c r="A12" s="21"/>
+      <c r="A12" s="22"/>
       <c r="C12" s="2" t="s">
         <v>21</v>
       </c>
@@ -844,7 +847,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="45">
-      <c r="A13" s="21"/>
+      <c r="A13" s="22"/>
       <c r="C13" s="10" t="s">
         <v>22</v>
       </c>
@@ -876,7 +879,7 @@
       <c r="D16" s="15"/>
     </row>
     <row r="17" spans="1:4" ht="64">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="13" t="s">
@@ -887,7 +890,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="32">
-      <c r="A18" s="21"/>
+      <c r="A18" s="22"/>
       <c r="C18" s="5" t="s">
         <v>25</v>
       </c>
@@ -896,7 +899,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="32">
-      <c r="A19" s="21"/>
+      <c r="A19" s="22"/>
       <c r="C19" s="13" t="s">
         <v>26</v>
       </c>
@@ -905,7 +908,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="64">
-      <c r="A20" s="21"/>
+      <c r="A20" s="22"/>
       <c r="C20" s="5" t="s">
         <v>27</v>
       </c>
@@ -914,7 +917,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="16">
-      <c r="A21" s="21"/>
+      <c r="A21" s="22"/>
       <c r="C21" s="5" t="s">
         <v>28</v>
       </c>
@@ -923,7 +926,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="32">
-      <c r="A22" s="21"/>
+      <c r="A22" s="22"/>
       <c r="C22" s="5" t="s">
         <v>29</v>
       </c>
@@ -938,7 +941,7 @@
       <c r="D23" s="15"/>
     </row>
     <row r="24" spans="1:4" ht="64">
-      <c r="A24" s="21" t="s">
+      <c r="A24" s="22" t="s">
         <v>13</v>
       </c>
       <c r="C24" s="4" t="s">
@@ -949,7 +952,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="32">
-      <c r="A25" s="21"/>
+      <c r="A25" s="22"/>
       <c r="C25" s="4" t="s">
         <v>30</v>
       </c>
@@ -958,7 +961,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="48">
-      <c r="A26" s="21"/>
+      <c r="A26" s="22"/>
       <c r="C26" s="4" t="s">
         <v>31</v>
       </c>
@@ -990,7 +993,7 @@
       <c r="D29" s="15"/>
     </row>
     <row r="30" spans="1:4" ht="32">
-      <c r="A30" s="21" t="s">
+      <c r="A30" s="22" t="s">
         <v>34</v>
       </c>
       <c r="C30" s="4" t="s">
@@ -1001,7 +1004,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="96">
-      <c r="A31" s="21"/>
+      <c r="A31" s="22"/>
       <c r="C31" s="14" t="s">
         <v>36</v>
       </c>
@@ -1016,7 +1019,7 @@
       <c r="D32" s="15"/>
     </row>
     <row r="33" spans="1:4" ht="32">
-      <c r="A33" s="21" t="s">
+      <c r="A33" s="22" t="s">
         <v>37</v>
       </c>
       <c r="C33" s="4" t="s">
@@ -1027,7 +1030,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="32">
-      <c r="A34" s="21"/>
+      <c r="A34" s="22"/>
       <c r="C34" s="4" t="s">
         <v>39</v>
       </c>
@@ -1036,7 +1039,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="32">
-      <c r="A35" s="21"/>
+      <c r="A35" s="22"/>
       <c r="C35" s="4" t="s">
         <v>40</v>
       </c>
@@ -1045,7 +1048,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="144">
-      <c r="A36" s="21"/>
+      <c r="A36" s="22"/>
       <c r="C36" s="4" t="s">
         <v>41</v>
       </c>
@@ -1060,7 +1063,7 @@
       <c r="D37" s="15"/>
     </row>
     <row r="38" spans="1:4" ht="80">
-      <c r="A38" s="21" t="s">
+      <c r="A38" s="22" t="s">
         <v>42</v>
       </c>
       <c r="C38" s="4" t="s">
@@ -1071,7 +1074,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="64">
-      <c r="A39" s="21"/>
+      <c r="A39" s="22"/>
       <c r="C39" s="4" t="s">
         <v>44</v>
       </c>
@@ -1080,7 +1083,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="48">
-      <c r="A40" s="21"/>
+      <c r="A40" s="22"/>
       <c r="C40" s="4" t="s">
         <v>45</v>
       </c>
@@ -1117,10 +1120,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>
@@ -1129,9 +1132,10 @@
     <col min="2" max="2" width="10.83203125" style="9"/>
     <col min="3" max="3" width="93" style="2" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="16"/>
+    <col min="5" max="5" width="47.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -1142,8 +1146,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="136">
-      <c r="A2" s="21" t="s">
+    <row r="2" spans="1:5" ht="136">
+      <c r="A2" s="22" t="s">
         <v>48</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1152,9 +1156,12 @@
       <c r="D2" s="16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="48">
-      <c r="A3" s="21"/>
+      <c r="E2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="48">
+      <c r="A3" s="22"/>
       <c r="C3" s="4" t="s">
         <v>50</v>
       </c>
@@ -1162,43 +1169,43 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="8" customFormat="1">
+    <row r="4" spans="1:5" s="8" customFormat="1">
       <c r="A4" s="19"/>
       <c r="B4" s="6"/>
-      <c r="C4" s="23"/>
+      <c r="C4" s="21"/>
       <c r="D4" s="15"/>
     </row>
-    <row r="5" spans="1:4" ht="16">
-      <c r="A5" s="21" t="s">
+    <row r="5" spans="1:5" ht="16">
+      <c r="A5" s="22" t="s">
         <v>52</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="22"/>
-    </row>
-    <row r="6" spans="1:4" ht="16">
-      <c r="A6" s="21"/>
+      <c r="D5" s="23"/>
+    </row>
+    <row r="6" spans="1:5" ht="16">
+      <c r="A6" s="22"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="22"/>
-    </row>
-    <row r="7" spans="1:4" ht="16">
-      <c r="A7" s="21"/>
+      <c r="D6" s="23"/>
+    </row>
+    <row r="7" spans="1:5" ht="16">
+      <c r="A7" s="22"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="22"/>
-    </row>
-    <row r="8" spans="1:4" ht="15">
-      <c r="A8" s="21"/>
-      <c r="D8" s="22"/>
-    </row>
-    <row r="9" spans="1:4" s="8" customFormat="1">
+      <c r="D7" s="23"/>
+    </row>
+    <row r="8" spans="1:5" ht="15">
+      <c r="A8" s="22"/>
+      <c r="D8" s="23"/>
+    </row>
+    <row r="9" spans="1:5" s="8" customFormat="1">
       <c r="A9" s="19"/>
       <c r="B9" s="9"/>
       <c r="C9" s="7"/>
       <c r="D9" s="15"/>
     </row>
-    <row r="10" spans="1:4" ht="99" customHeight="1">
-      <c r="A10" s="21" t="s">
+    <row r="10" spans="1:5" ht="99" customHeight="1">
+      <c r="A10" s="22" t="s">
         <v>53</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1208,8 +1215,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="64">
-      <c r="A11" s="21"/>
+    <row r="11" spans="1:5" ht="64">
+      <c r="A11" s="22"/>
       <c r="C11" s="4" t="s">
         <v>55</v>
       </c>
@@ -1217,8 +1224,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="64">
-      <c r="A12" s="21"/>
+    <row r="12" spans="1:5" ht="64">
+      <c r="A12" s="22"/>
       <c r="C12" s="4" t="s">
         <v>56</v>
       </c>
@@ -1226,8 +1233,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="48">
-      <c r="A13" s="21"/>
+    <row r="13" spans="1:5" ht="48">
+      <c r="A13" s="22"/>
       <c r="C13" s="4" t="s">
         <v>57</v>
       </c>
@@ -1235,14 +1242,14 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="8" customFormat="1">
+    <row r="14" spans="1:5" s="8" customFormat="1">
       <c r="A14" s="19"/>
       <c r="B14" s="6"/>
       <c r="C14" s="7"/>
       <c r="D14" s="15"/>
     </row>
-    <row r="15" spans="1:4" ht="96">
-      <c r="A15" s="21" t="s">
+    <row r="15" spans="1:5" ht="96">
+      <c r="A15" s="22" t="s">
         <v>59</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -1252,8 +1259,8 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="32">
-      <c r="A16" s="21"/>
+    <row r="16" spans="1:5" ht="32">
+      <c r="A16" s="22"/>
       <c r="C16" s="4" t="s">
         <v>62</v>
       </c>
@@ -1262,7 +1269,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="160">
-      <c r="A17" s="21"/>
+      <c r="A17" s="22"/>
       <c r="C17" s="4" t="s">
         <v>63</v>
       </c>
@@ -1271,7 +1278,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="48">
-      <c r="A18" s="21"/>
+      <c r="A18" s="22"/>
       <c r="C18" s="4" t="s">
         <v>64</v>
       </c>

</xml_diff>